<commit_message>
[CODE] finalisation changement de features
</commit_message>
<xml_diff>
--- a/admin/features_files/template/Template_Features.xlsx
+++ b/admin/features_files/template/Template_Features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nom de la feature (Texte affiché sur la carte lors de la phase de classement)</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Question affichée en haut de la page lors de la phase de classement</t>
+  </si>
+  <si>
+    <t>Question affichée dans la partie de QCM introductif</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -417,7 +420,7 @@
     <col min="1" max="16384" width="32.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -429,6 +432,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -479,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.42578125" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>